<commit_message>
3 selenium tests added
</commit_message>
<xml_diff>
--- a/Bulls_Cows_TestCases.xlsx
+++ b/Bulls_Cows_TestCases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Julia\Programming\Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Julia\Programming\Testing\Bulls_Cows_codepen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{03BB2C52-3446-469A-B2D7-9E072CAADBFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB70694F-74DD-4399-BD39-DCDACECDE693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case 1" sheetId="7" r:id="rId1"/>
@@ -22,21 +22,11 @@
     <sheet name="Test Case 7" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="80000"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="72">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -188,15 +178,6 @@
     <t>BC_005</t>
   </si>
   <si>
-    <t>All numbers starting from 1000 to 9999</t>
-  </si>
-  <si>
-    <t>Verify if secret number exists and there is only one secret number</t>
-  </si>
-  <si>
-    <t>Test the existence and uniqueness of  the secret number (for automated testing only)</t>
-  </si>
-  <si>
     <t>Test the error messaging with an invalid number (too short)</t>
   </si>
   <si>
@@ -248,13 +229,25 @@
     <t>Test BC_001 passes</t>
   </si>
   <si>
-    <t>For the rest of numbers from Test Data do the following steps: 1. Enter Number 2. Click Submit</t>
+    <t>All numbers containing different digits starting from 1023 to 9876</t>
+  </si>
+  <si>
+    <t>Verify if secret number exists</t>
+  </si>
+  <si>
+    <t>Test the existence of  the secret number (for automated testing only)</t>
+  </si>
+  <si>
+    <t>Execute test BC_001 with the rest of numbers from Test Data</t>
+  </si>
+  <si>
+    <t>Execute test BC_001 with the rest of numbers from Test Data until the secret number is found</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
@@ -520,6 +513,10 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -529,85 +526,81 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -889,10 +882,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -902,46 +895,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="44" t="s">
+      <c r="E1" s="41"/>
+      <c r="F1" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="42" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="37"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -957,10 +950,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -985,29 +978,29 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="26" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="22"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -1026,100 +1019,100 @@
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="9"/>
       <c r="F8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="3"/>
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="3"/>
       <c r="F10" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>3</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="3"/>
       <c r="F11" s="11">
         <v>3</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>4</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="3"/>
       <c r="F12" s="11">
         <v>4</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -1130,13 +1123,13 @@
       <c r="F13" s="11">
         <v>5</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="19"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
@@ -1156,177 +1149,173 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>1</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17" t="s">
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>2</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="25" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="17" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="17" t="s">
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>3</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="17" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="17" t="s">
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>4</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="G11:K11"/>
     <mergeCell ref="B12:D12"/>
@@ -1337,26 +1326,30 @@
     <mergeCell ref="F16:H17"/>
     <mergeCell ref="I16:K17"/>
     <mergeCell ref="G13:K13"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1365,7 +1358,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
@@ -1378,46 +1371,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="42" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="37"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -1433,10 +1426,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1461,29 +1454,29 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="26" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="22"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -1502,96 +1495,96 @@
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="9"/>
       <c r="F8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="3"/>
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="3"/>
       <c r="F10" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>3</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="3"/>
       <c r="F11" s="11">
         <v>3</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>4</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="3"/>
       <c r="F12" s="11">
         <v>4</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -1611,7 +1604,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -1624,169 +1617,165 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>1</v>
       </c>
-      <c r="B18" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="17" t="s">
+      <c r="B18" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17" t="s">
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>2</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="25" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="17" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="17" t="s">
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>3</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>4</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="G11:K11"/>
     <mergeCell ref="B12:D12"/>
@@ -1796,26 +1785,30 @@
     <mergeCell ref="D16:E17"/>
     <mergeCell ref="F16:H17"/>
     <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1824,11 +1817,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:E18"/>
+      <selection activeCell="B19" sqref="B19:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1837,46 +1830,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="44" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="42" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="37"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -1892,10 +1885,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -1920,29 +1913,29 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="26" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="22"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -1961,94 +1954,94 @@
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="9"/>
       <c r="F8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="3"/>
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="G9" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="3"/>
       <c r="F10" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>3</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="3"/>
       <c r="F11" s="11">
         <v>3</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>4</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="3"/>
       <c r="F12" s="11">
         <v>4</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -2068,7 +2061,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -2081,169 +2074,165 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>1</v>
       </c>
-      <c r="B18" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="17" t="s">
+      <c r="B18" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="E18" s="17"/>
+      <c r="F18" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17" t="s">
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>2</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="17" t="s">
+      <c r="B19" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="17"/>
+      <c r="F19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="17" t="s">
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>3</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="17"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="B20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="17"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>4</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="G11:K11"/>
     <mergeCell ref="B12:D12"/>
@@ -2253,26 +2242,30 @@
     <mergeCell ref="D16:E17"/>
     <mergeCell ref="F16:H17"/>
     <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2281,11 +2274,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:E18"/>
+      <selection activeCell="B18" sqref="B18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2294,46 +2287,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="44" t="s">
-        <v>53</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="42" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="37"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -2349,10 +2342,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -2377,29 +2370,29 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="26" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="K6" s="22"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -2418,94 +2411,94 @@
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="9"/>
       <c r="F8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="3"/>
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="3"/>
       <c r="F10" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>3</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="3"/>
       <c r="F11" s="11">
         <v>3</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>4</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="3"/>
       <c r="F12" s="11">
         <v>4</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -2538,177 +2531,173 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>1</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="21"/>
+      <c r="D18" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="21"/>
+      <c r="F18" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17" t="s">
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>2</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="25" t="s">
+      <c r="C19" s="21"/>
+      <c r="D19" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="17" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="17" t="s">
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>3</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="17" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="17" t="s">
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>4</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="G11:K11"/>
     <mergeCell ref="B12:D12"/>
@@ -2718,26 +2707,30 @@
     <mergeCell ref="D16:E17"/>
     <mergeCell ref="F16:H17"/>
     <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -2746,11 +2739,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:E18"/>
+      <selection activeCell="B18" sqref="B18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2759,46 +2752,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="42" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="37"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -2814,10 +2807,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -2842,29 +2835,29 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="26" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="22"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -2883,94 +2876,94 @@
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="9"/>
       <c r="F8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="3"/>
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="G9" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="3"/>
       <c r="F10" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>3</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="3"/>
       <c r="F11" s="11">
         <v>3</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>4</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="3"/>
       <c r="F12" s="11">
         <v>4</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -2990,7 +2983,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3003,177 +2996,173 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>1</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="21"/>
+      <c r="D18" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="21"/>
+      <c r="F18" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17" t="s">
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>2</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="25" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="17" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="17" t="s">
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
     </row>
     <row r="20" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>3</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="17" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="17" t="s">
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>4</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="G11:K11"/>
     <mergeCell ref="B12:D12"/>
@@ -3183,26 +3172,30 @@
     <mergeCell ref="D16:E17"/>
     <mergeCell ref="F16:H17"/>
     <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -3211,11 +3204,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B18" sqref="B18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3224,46 +3217,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="44" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="42" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="37"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -3279,10 +3272,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -3307,29 +3300,29 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="26" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="22"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -3348,94 +3341,94 @@
       <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="9"/>
       <c r="F8" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="3"/>
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="G9" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="3"/>
       <c r="F10" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>3</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="3"/>
       <c r="F11" s="11">
         <v>3</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>4</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="3"/>
       <c r="F12" s="11">
         <v>4</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -3455,7 +3448,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3468,177 +3461,173 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>1</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="21"/>
+      <c r="D18" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="21"/>
+      <c r="F18" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17" t="s">
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>2</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="25" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="17" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="17" t="s">
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
     </row>
     <row r="20" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>3</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="17" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="17" t="s">
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>4</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:H22"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I23:K23"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:H20"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:H21"/>
-    <mergeCell ref="I21:K21"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="I18:K18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:H19"/>
-    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="G11:K11"/>
     <mergeCell ref="B12:D12"/>
@@ -3648,26 +3637,30 @@
     <mergeCell ref="D16:E17"/>
     <mergeCell ref="F16:H17"/>
     <mergeCell ref="I16:K17"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="G10:K10"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="I18:K18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:H21"/>
+    <mergeCell ref="I21:K21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I23:K23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -3676,10 +3669,10 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -3689,46 +3682,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="46"/>
+      <c r="B1" s="41"/>
       <c r="C1" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D1" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="19"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="21"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="46"/>
+      <c r="B2" s="41"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="45" t="s">
+      <c r="D2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="46"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="42" t="s">
+      <c r="E2" s="41"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="43"/>
-      <c r="J2" s="41" t="s">
+      <c r="I2" s="45"/>
+      <c r="J2" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="37"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -3744,10 +3737,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="13"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -3772,29 +3765,29 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="27"/>
-      <c r="F6" s="39" t="s">
+      <c r="E6" s="35"/>
+      <c r="F6" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="40"/>
-      <c r="H6" s="26" t="s">
+      <c r="G6" s="38"/>
+      <c r="H6" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="22" t="s">
+      <c r="I6" s="35"/>
+      <c r="J6" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="22"/>
+      <c r="K6" s="39"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -3813,94 +3806,94 @@
       <c r="A8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="9"/>
       <c r="F8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="18"/>
-      <c r="D9" s="19"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="21"/>
       <c r="E9" s="3"/>
       <c r="F9" s="11">
         <v>1</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="19"/>
+      <c r="G9" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="21"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="21"/>
       <c r="E10" s="3"/>
       <c r="F10" s="11">
         <v>2</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="21"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>3</v>
       </c>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="21"/>
       <c r="E11" s="3"/>
       <c r="F11" s="11">
         <v>3</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="K11" s="19"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>4</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="3"/>
       <c r="F12" s="11">
         <v>4</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18"/>
-      <c r="K12" s="19"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
@@ -3920,7 +3913,7 @@
         <v>20</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
@@ -3933,163 +3926,174 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="28" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="29"/>
-      <c r="F16" s="20" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="20" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="21"/>
-      <c r="K16" s="21"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
-      <c r="K17" s="21"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11">
         <v>1</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="22"/>
+      <c r="D18" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="25"/>
-      <c r="F18" s="17" t="s">
+      <c r="E18" s="17"/>
+      <c r="F18" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G18" s="18"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="17" t="s">
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J18" s="18"/>
-      <c r="K18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="11">
         <v>2</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="25" t="s">
+      <c r="C19" s="18"/>
+      <c r="D19" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="25"/>
-      <c r="F19" s="17" t="s">
+      <c r="E19" s="17"/>
+      <c r="F19" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="17" t="s">
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="J19" s="18"/>
-      <c r="K19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21"/>
     </row>
     <row r="20" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11">
         <v>3</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="25" t="s">
+      <c r="C20" s="18"/>
+      <c r="D20" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="E20" s="25"/>
-      <c r="F20" s="17" t="s">
+      <c r="E20" s="17"/>
+      <c r="F20" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="18"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="17" t="s">
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11">
         <v>4</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="17"/>
-      <c r="G21" s="18"/>
-      <c r="H21" s="19"/>
-      <c r="I21" s="17"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="19"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
-      <c r="B22" s="25"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="19"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
-      <c r="B23" s="25"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="19"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="53">
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:H23"/>
+    <mergeCell ref="I19:K19"/>
+    <mergeCell ref="I20:K20"/>
+    <mergeCell ref="F16:H17"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="I23:K23"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="G11:K11"/>
+    <mergeCell ref="G12:K12"/>
+    <mergeCell ref="D16:E17"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="F19:H19"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="I16:K17"/>
+    <mergeCell ref="G9:K9"/>
+    <mergeCell ref="G10:K10"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="D2:E2"/>
@@ -4106,33 +4110,22 @@
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D23:E23"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="B16:C17"/>
     <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="G11:K11"/>
-    <mergeCell ref="G12:K12"/>
-    <mergeCell ref="D16:E17"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="F19:H19"/>
     <mergeCell ref="F20:H20"/>
     <mergeCell ref="F21:H21"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="G8:K8"/>
-    <mergeCell ref="I16:K17"/>
-    <mergeCell ref="G9:K9"/>
-    <mergeCell ref="G10:K10"/>
     <mergeCell ref="F22:H22"/>
-    <mergeCell ref="F23:H23"/>
-    <mergeCell ref="I19:K19"/>
-    <mergeCell ref="I20:K20"/>
-    <mergeCell ref="F16:H17"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="I22:K22"/>
-    <mergeCell ref="I23:K23"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>